<commit_message>
sigmoid fn for prob fix
</commit_message>
<xml_diff>
--- a/logi-reg/Project3-logi-reg.xlsx
+++ b/logi-reg/Project3-logi-reg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denni\src\repo\data-sci\student-grade-regression\logi-reg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D724DE-3DE2-480D-96C0-D4DAF0D3DFFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE7989B-6044-432D-B2E9-95C72CB3BD50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2310" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Midterm</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>x0</t>
+  </si>
+  <si>
+    <t>pass prob</t>
   </si>
 </sst>
 </file>
@@ -104,7 +107,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -116,6 +119,7 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E332"/>
   <sheetViews>
-    <sheetView topLeftCell="A307" workbookViewId="0">
-      <selection activeCell="E332" sqref="E332"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6119,1015 +6123,1183 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="L1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
         <v>49</v>
       </c>
-      <c r="B2" s="3">
+      <c r="C2" s="3">
         <v>79</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="3">
         <v>71</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2">
-        <v>4.1999999999999997E-3</v>
-      </c>
-      <c r="G2">
-        <v>0.34839999999999999</v>
-      </c>
-      <c r="H2">
-        <v>0.35770000000000002</v>
+      <c r="G2" s="5">
+        <v>-0.21340000000000001</v>
+      </c>
+      <c r="H2" s="5">
+        <v>-6.54E-2</v>
       </c>
       <c r="I2">
-        <v>0.35370000000000001</v>
-      </c>
-      <c r="K2">
-        <f>SUMPRODUCT($F$2:$I$2, A2:D2)</f>
-        <v>53.126100000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+        <v>1.8100000000000002E-2</v>
+      </c>
+      <c r="J2">
+        <v>7.9200000000000007E-2</v>
+      </c>
+      <c r="L2">
+        <f>EXP(SUMPRODUCT($G$2:$J$2, A2:D2))/(1+EXP(SUMPRODUCT($G$2:$J$2, A2:D2)))</f>
+        <v>0.974296787923282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
         <v>56</v>
       </c>
-      <c r="B3" s="3">
+      <c r="C3" s="3">
         <v>21</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="3">
         <v>46</v>
       </c>
-      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="K3">
-        <f>SUMPRODUCT($F$2:$I$2, A3:D3)</f>
-        <v>24.005800000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="L3">
+        <f>EXP(SUMPRODUCT($G$2:$J$2, A3:D3))/(1+EXP(SUMPRODUCT($G$2:$J$2, A3:D3)))</f>
+        <v>0.53680828998898056</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
         <v>58</v>
       </c>
-      <c r="B4" s="3">
+      <c r="C4" s="3">
         <v>100</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="3">
         <v>79</v>
       </c>
-      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="K4">
-        <f t="shared" ref="K4:K55" si="0">SUMPRODUCT($F$2:$I$2, A4:D4)</f>
-        <v>63.341899999999995</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="H4" s="1"/>
+      <c r="L4">
+        <f t="shared" ref="L4:L55" si="0">EXP(SUMPRODUCT($G$2:$J$2, A4:D4))/(1+EXP(SUMPRODUCT($G$2:$J$2, A4:D4)))</f>
+        <v>0.9830467979700277</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
         <v>61</v>
       </c>
-      <c r="B5" s="3">
+      <c r="C5" s="3">
         <v>82</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="3">
         <v>58</v>
       </c>
-      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="K5">
+      <c r="H5" s="1"/>
+      <c r="L5">
         <f t="shared" si="0"/>
-        <v>49.571600000000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+        <v>0.86703575980217085</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3">
         <v>62</v>
       </c>
-      <c r="B6" s="3">
+      <c r="C6" s="3">
         <v>90</v>
       </c>
-      <c r="C6" s="3">
+      <c r="D6" s="3">
         <v>62</v>
       </c>
-      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="K6">
+      <c r="H6" s="1"/>
+      <c r="L6">
         <f t="shared" si="0"/>
-        <v>53.793800000000005</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+        <v>0.90646358222852741</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
         <v>66</v>
       </c>
-      <c r="B7" s="3">
+      <c r="C7" s="3">
         <v>99</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="3">
         <v>75</v>
       </c>
-      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="K7">
+      <c r="H7" s="1"/>
+      <c r="L7">
         <f t="shared" si="0"/>
-        <v>61.596299999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+        <v>0.96091322748473462</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3">
         <v>71</v>
       </c>
-      <c r="B8" s="3">
+      <c r="C8" s="3">
         <v>73</v>
       </c>
-      <c r="C8" s="3">
+      <c r="D8" s="3">
         <v>65</v>
       </c>
-      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="K8">
+      <c r="H8" s="1"/>
+      <c r="L8">
         <f t="shared" si="0"/>
-        <v>48.981900000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+        <v>0.83375818929235768</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3">
         <v>73</v>
       </c>
-      <c r="B9" s="3">
+      <c r="C9" s="3">
         <v>87</v>
       </c>
-      <c r="C9" s="3">
+      <c r="D9" s="3">
         <v>80</v>
       </c>
-      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="K9">
+      <c r="H9" s="1"/>
+      <c r="L9">
         <f t="shared" si="0"/>
-        <v>59.233400000000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+        <v>0.9489766101805357</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3">
         <v>73</v>
       </c>
-      <c r="B10" s="3">
+      <c r="C10" s="3">
         <v>97</v>
       </c>
-      <c r="C10" s="3">
+      <c r="D10" s="3">
         <v>73</v>
       </c>
-      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="K10">
+      <c r="H10" s="1"/>
+      <c r="L10">
         <f t="shared" si="0"/>
-        <v>60.21350000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+        <v>0.92755335778619874</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3">
         <v>74</v>
       </c>
-      <c r="B11" s="3">
+      <c r="C11" s="3">
         <v>73</v>
       </c>
-      <c r="C11" s="3">
+      <c r="D11" s="3">
         <v>77</v>
       </c>
-      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="K11">
+      <c r="H11" s="1"/>
+      <c r="L11">
         <f t="shared" si="0"/>
-        <v>53.286900000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+        <v>0.91425251094349391</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3">
         <v>74</v>
       </c>
-      <c r="B12" s="3">
+      <c r="C12" s="3">
         <v>85</v>
       </c>
-      <c r="C12" s="3">
+      <c r="D12" s="3">
         <v>66</v>
       </c>
-      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="K12">
+      <c r="H12" s="1"/>
+      <c r="L12">
         <f t="shared" si="0"/>
-        <v>53.533000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+        <v>0.8471861587777948</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3">
         <v>74</v>
       </c>
-      <c r="B13" s="3">
+      <c r="C13" s="3">
         <v>100</v>
       </c>
-      <c r="C13" s="3">
+      <c r="D13" s="3">
         <v>87</v>
       </c>
-      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="K13">
+      <c r="H13" s="1"/>
+      <c r="L13">
         <f t="shared" si="0"/>
-        <v>66.270700000000005</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+        <v>0.97460302099517893</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3">
         <v>78</v>
       </c>
-      <c r="B14" s="3">
+      <c r="C14" s="3">
         <v>79</v>
       </c>
-      <c r="C14" s="3">
+      <c r="D14" s="3">
         <v>56</v>
       </c>
-      <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="K14">
+      <c r="H14" s="1"/>
+      <c r="L14">
         <f t="shared" si="0"/>
-        <v>47.882400000000004</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+        <v>0.63425158705039753</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3">
         <v>80</v>
       </c>
-      <c r="B15" s="3">
+      <c r="C15" s="3">
         <v>72</v>
       </c>
-      <c r="C15" s="3">
+      <c r="D15" s="3">
         <v>71</v>
       </c>
-      <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="K15">
+      <c r="H15" s="1"/>
+      <c r="L15">
         <f t="shared" si="0"/>
-        <v>50.817499999999995</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+        <v>0.81472357728651845</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3">
         <v>80</v>
       </c>
-      <c r="B16" s="3">
+      <c r="C16" s="3">
         <v>82</v>
       </c>
-      <c r="C16" s="3">
+      <c r="D16" s="3">
         <v>90</v>
       </c>
-      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="K16">
+      <c r="H16" s="1"/>
+      <c r="L16">
         <f t="shared" si="0"/>
-        <v>61.097800000000007</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+        <v>0.9595656087591683</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3">
         <v>81</v>
       </c>
-      <c r="B17" s="3">
+      <c r="C17" s="3">
         <v>80</v>
       </c>
-      <c r="C17" s="3">
+      <c r="D17" s="3">
         <v>78</v>
       </c>
-      <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="K17">
+      <c r="H17" s="1"/>
+      <c r="L17">
         <f t="shared" si="0"/>
-        <v>56.1128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+        <v>0.89233336020560505</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3">
         <v>81</v>
       </c>
-      <c r="B18" s="3">
+      <c r="C18" s="3">
         <v>56</v>
       </c>
-      <c r="C18" s="3">
+      <c r="D18" s="3">
         <v>60</v>
       </c>
-      <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="K18">
+      <c r="H18" s="1"/>
+      <c r="L18">
         <f t="shared" si="0"/>
-        <v>41.312600000000003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+        <v>0.56335758972258787</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3">
         <v>82</v>
       </c>
-      <c r="B19" s="3">
+      <c r="C19" s="3">
         <v>100</v>
       </c>
-      <c r="C19" s="3">
+      <c r="D19" s="3">
         <v>79</v>
       </c>
-      <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="K19">
+      <c r="H19" s="1"/>
+      <c r="L19">
         <f t="shared" si="0"/>
-        <v>63.442700000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+        <v>0.9234802121286223</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3">
         <v>83</v>
       </c>
-      <c r="B20" s="3">
+      <c r="C20" s="3">
         <v>80</v>
       </c>
-      <c r="C20" s="3">
+      <c r="D20" s="3">
         <v>56</v>
       </c>
-      <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="K20">
+      <c r="H20" s="1"/>
+      <c r="L20">
         <f t="shared" si="0"/>
-        <v>48.251800000000003</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+        <v>0.56010790636318275</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" s="3">
         <v>83</v>
       </c>
-      <c r="B21" s="3">
+      <c r="C21" s="3">
         <v>96</v>
       </c>
-      <c r="C21" s="3">
+      <c r="D21" s="3">
         <v>64</v>
       </c>
-      <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="K21">
+      <c r="H21" s="1"/>
+      <c r="L21">
         <f t="shared" si="0"/>
-        <v>56.687799999999996</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+        <v>0.76220380549522238</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" s="3">
         <v>84</v>
       </c>
-      <c r="B22" s="3">
+      <c r="C22" s="3">
         <v>98</v>
       </c>
-      <c r="C22" s="3">
+      <c r="D22" s="3">
         <v>85</v>
       </c>
-      <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="K22">
+      <c r="H22" s="1"/>
+      <c r="L22">
         <f t="shared" si="0"/>
-        <v>64.900500000000008</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+        <v>0.94261094390613664</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3">
         <v>84</v>
       </c>
-      <c r="B23" s="3">
+      <c r="C23" s="3">
         <v>100</v>
       </c>
-      <c r="C23" s="3">
+      <c r="D23" s="3">
         <v>77</v>
       </c>
-      <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="K23">
+      <c r="H23" s="1"/>
+      <c r="L23">
         <f t="shared" si="0"/>
-        <v>62.735700000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+        <v>0.90037516091253866</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" s="3">
         <v>85</v>
       </c>
-      <c r="B24" s="3">
+      <c r="C24" s="3">
         <v>93</v>
       </c>
-      <c r="C24" s="3">
+      <c r="D24" s="3">
         <v>75</v>
       </c>
-      <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="K24">
+      <c r="H24" s="1"/>
+      <c r="L24">
         <f t="shared" si="0"/>
-        <v>59.585699999999996</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+        <v>0.86423273867302264</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" s="3">
         <v>85</v>
       </c>
-      <c r="B25" s="3">
+      <c r="C25" s="3">
         <v>99</v>
       </c>
-      <c r="C25" s="3">
+      <c r="D25" s="3">
         <v>69</v>
       </c>
-      <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="K25">
+      <c r="H25" s="1"/>
+      <c r="L25">
         <f t="shared" si="0"/>
-        <v>59.529899999999998</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+        <v>0.81522119194908294</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" s="3">
         <v>86</v>
       </c>
-      <c r="B26" s="3">
+      <c r="C26" s="3">
         <v>100</v>
       </c>
-      <c r="C26" s="3">
+      <c r="D26" s="3">
         <v>85</v>
       </c>
-      <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="K26">
+      <c r="H26" s="1"/>
+      <c r="L26">
         <f t="shared" si="0"/>
-        <v>65.605699999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+        <v>0.93727402190659337</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" s="3">
         <v>86</v>
       </c>
-      <c r="B27" s="3">
+      <c r="C27" s="3">
         <v>95</v>
       </c>
-      <c r="C27" s="3">
+      <c r="D27" s="3">
         <v>77</v>
       </c>
-      <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="K27">
+      <c r="H27" s="1"/>
+      <c r="L27">
         <f t="shared" si="0"/>
-        <v>61.002099999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+        <v>0.87869182176233973</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" s="3">
         <v>87</v>
       </c>
-      <c r="B28" s="3">
+      <c r="C28" s="3">
         <v>98</v>
       </c>
-      <c r="C28" s="3">
+      <c r="D28" s="3">
         <v>89</v>
       </c>
-      <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="K28">
+      <c r="H28" s="1"/>
+      <c r="L28">
         <f t="shared" si="0"/>
-        <v>66.343900000000005</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+        <v>0.9487971582643322</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" s="3">
         <v>87</v>
       </c>
-      <c r="B29" s="3">
+      <c r="C29" s="3">
         <v>99</v>
       </c>
-      <c r="C29" s="3">
+      <c r="D29" s="3">
         <v>85</v>
       </c>
-      <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="K29">
+      <c r="H29" s="1"/>
+      <c r="L29">
         <f t="shared" si="0"/>
-        <v>65.261499999999998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
+        <v>0.93218197293261962</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" s="3">
         <v>87</v>
       </c>
-      <c r="B30" s="3">
+      <c r="C30" s="3">
         <v>99</v>
       </c>
-      <c r="C30" s="3">
+      <c r="D30" s="3">
         <v>90</v>
       </c>
-      <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="K30">
+      <c r="H30" s="1"/>
+      <c r="L30">
         <f t="shared" si="0"/>
-        <v>67.050000000000011</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
+        <v>0.95332290041612366</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" s="3">
         <v>87</v>
       </c>
-      <c r="B31" s="3">
+      <c r="C31" s="3">
         <v>97</v>
       </c>
-      <c r="C31" s="3">
+      <c r="D31" s="3">
         <v>75</v>
       </c>
-      <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="K31">
+      <c r="H31" s="1"/>
+      <c r="L31">
         <f t="shared" si="0"/>
-        <v>60.987700000000004</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
+        <v>0.85723351040055018</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" s="3">
         <v>87</v>
       </c>
-      <c r="B32" s="3">
+      <c r="C32" s="3">
         <v>99</v>
       </c>
-      <c r="C32" s="3">
+      <c r="D32" s="3">
         <v>81</v>
       </c>
-      <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="K32">
+      <c r="H32" s="1"/>
+      <c r="L32">
         <f t="shared" si="0"/>
-        <v>63.8307</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
+        <v>0.90919952065180132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" s="3">
         <v>88</v>
       </c>
-      <c r="B33" s="3">
+      <c r="C33" s="3">
         <v>99</v>
       </c>
-      <c r="C33" s="3">
+      <c r="D33" s="3">
         <v>73</v>
       </c>
-      <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="K33">
+      <c r="H33" s="1"/>
+      <c r="L33">
         <f t="shared" si="0"/>
-        <v>60.973299999999995</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
+        <v>0.83270211399466365</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" s="3">
         <v>89</v>
       </c>
-      <c r="B34" s="3">
+      <c r="C34" s="3">
         <v>99</v>
       </c>
-      <c r="C34" s="3">
+      <c r="D34" s="3">
         <v>64</v>
       </c>
-      <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="K34">
+      <c r="H34" s="1"/>
+      <c r="L34">
         <f t="shared" si="0"/>
-        <v>57.758200000000002</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
+        <v>0.69565671038427057</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" s="3">
         <v>89</v>
       </c>
-      <c r="B35" s="3">
+      <c r="C35" s="3">
         <v>82</v>
       </c>
-      <c r="C35" s="3">
+      <c r="D35" s="3">
         <v>37</v>
       </c>
-      <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="K35">
+      <c r="H35" s="1"/>
+      <c r="L35">
         <f t="shared" si="0"/>
-        <v>42.177500000000002</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
+        <v>0.16528763414614689</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" s="3">
         <v>89</v>
       </c>
-      <c r="B36" s="3">
+      <c r="C36" s="3">
         <v>82</v>
       </c>
-      <c r="C36" s="3">
+      <c r="D36" s="3">
         <v>81</v>
       </c>
-      <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-      <c r="K36">
+      <c r="H36" s="1"/>
+      <c r="L36">
         <f t="shared" si="0"/>
-        <v>57.9163</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
+        <v>0.86592512133929933</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" s="3">
         <v>89</v>
       </c>
-      <c r="B37" s="3">
+      <c r="C37" s="3">
         <v>99</v>
       </c>
-      <c r="C37" s="3">
+      <c r="D37" s="3">
         <v>79</v>
       </c>
-      <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-      <c r="K37">
+      <c r="H37" s="1"/>
+      <c r="L37">
         <f t="shared" si="0"/>
-        <v>63.123699999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
+        <v>0.88233186474369951</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" s="3">
         <v>90</v>
       </c>
-      <c r="B38" s="3">
+      <c r="C38" s="3">
         <v>100</v>
       </c>
-      <c r="C38" s="3">
+      <c r="D38" s="3">
         <v>90</v>
       </c>
-      <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-      <c r="K38">
+      <c r="H38" s="1"/>
+      <c r="L38">
         <f t="shared" si="0"/>
-        <v>67.411000000000001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
+        <v>0.94472640191916923</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" s="3">
         <v>91</v>
       </c>
-      <c r="B39" s="3">
+      <c r="C39" s="3">
         <v>100</v>
       </c>
-      <c r="C39" s="3">
+      <c r="D39" s="3">
         <v>79</v>
       </c>
-      <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
-      <c r="K39">
+      <c r="H39" s="1"/>
+      <c r="L39">
         <f t="shared" si="0"/>
-        <v>63.480499999999992</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
+        <v>0.87011771874629984</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40" s="3">
         <v>91</v>
       </c>
-      <c r="B40" s="3">
+      <c r="C40" s="3">
         <v>67</v>
       </c>
-      <c r="C40" s="3">
+      <c r="D40" s="3">
         <v>84</v>
       </c>
-      <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="K40">
+      <c r="H40" s="1"/>
+      <c r="L40">
         <f t="shared" si="0"/>
-        <v>53.771799999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
+        <v>0.84562613682783494</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" s="3">
         <v>92</v>
       </c>
-      <c r="B41" s="3">
+      <c r="C41" s="3">
         <v>99</v>
       </c>
-      <c r="C41" s="3">
+      <c r="D41" s="3">
         <v>85</v>
       </c>
-      <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-      <c r="K41">
+      <c r="H41" s="1"/>
+      <c r="L41">
         <f t="shared" si="0"/>
-        <v>65.282499999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
+        <v>0.90835392995347097</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" s="3">
         <v>93</v>
       </c>
-      <c r="B42" s="3">
+      <c r="C42" s="3">
         <v>97</v>
       </c>
-      <c r="C42" s="3">
+      <c r="D42" s="3">
         <v>71</v>
       </c>
-      <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="K42">
+      <c r="H42" s="1"/>
+      <c r="L42">
         <f t="shared" si="0"/>
-        <v>59.582100000000004</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
+        <v>0.74711796956557552</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43" s="3">
         <v>94</v>
       </c>
-      <c r="B43" s="3">
+      <c r="C43" s="3">
         <v>99</v>
       </c>
-      <c r="C43" s="3">
+      <c r="D43" s="3">
         <v>89</v>
       </c>
-      <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-      <c r="K43">
+      <c r="H43" s="1"/>
+      <c r="L43">
         <f t="shared" si="0"/>
-        <v>66.721699999999998</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
+        <v>0.9227064047877922</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" s="3">
         <v>95</v>
       </c>
-      <c r="B44" s="3">
+      <c r="C44" s="3">
         <v>98</v>
       </c>
-      <c r="C44" s="3">
+      <c r="D44" s="3">
         <v>85</v>
       </c>
-      <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
-      <c r="K44">
+      <c r="H44" s="1"/>
+      <c r="L44">
         <f t="shared" si="0"/>
-        <v>64.946700000000007</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
+        <v>0.88888478594064679</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45" s="3">
         <v>95</v>
       </c>
-      <c r="B45" s="3">
+      <c r="C45" s="3">
         <v>99</v>
       </c>
-      <c r="C45" s="3">
+      <c r="D45" s="3">
         <v>69</v>
       </c>
-      <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
-      <c r="K45">
+      <c r="H45" s="1"/>
+      <c r="L45">
         <f t="shared" si="0"/>
-        <v>59.571899999999999</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
-        <v>97</v>
+        <v>0.69641835950939923</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1</v>
       </c>
       <c r="B46" s="3">
         <v>97</v>
       </c>
       <c r="C46" s="3">
+        <v>97</v>
+      </c>
+      <c r="D46" s="3">
         <v>85</v>
       </c>
-      <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
-      <c r="K46">
+      <c r="H46" s="1"/>
+      <c r="L46">
         <f t="shared" si="0"/>
-        <v>64.606700000000004</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
+        <v>0.87330475198564839</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47" s="3">
         <v>97</v>
       </c>
-      <c r="B47" s="3">
+      <c r="C47" s="3">
         <v>80</v>
       </c>
-      <c r="C47" s="3">
+      <c r="D47" s="3">
         <v>79</v>
       </c>
-      <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
-      <c r="K47">
+      <c r="H47" s="1"/>
+      <c r="L47">
         <f t="shared" si="0"/>
-        <v>56.537700000000001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
+        <v>0.75907227415987577</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48" s="3">
         <v>97</v>
       </c>
-      <c r="B48" s="3">
+      <c r="C48" s="3">
         <v>99</v>
       </c>
-      <c r="C48" s="3">
+      <c r="D48" s="3">
         <v>92</v>
       </c>
-      <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
-      <c r="K48">
+      <c r="H48" s="1"/>
+      <c r="L48">
         <f t="shared" si="0"/>
-        <v>67.807400000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="3">
+        <v>0.92560783407252589</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49" s="3">
         <v>97</v>
       </c>
-      <c r="B49" s="3">
+      <c r="C49" s="3">
         <v>100</v>
       </c>
-      <c r="C49" s="3">
+      <c r="D49" s="3">
         <v>87</v>
       </c>
-      <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
-      <c r="K49">
+      <c r="H49" s="1"/>
+      <c r="L49">
         <f t="shared" si="0"/>
-        <v>66.3673</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="3">
+        <v>0.89503163077494385</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50" s="3">
         <v>98</v>
       </c>
-      <c r="B50" s="3">
+      <c r="C50" s="3">
         <v>100</v>
       </c>
-      <c r="C50" s="3">
+      <c r="D50" s="3">
         <v>81</v>
       </c>
-      <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
-      <c r="K50">
+      <c r="H50" s="1"/>
+      <c r="L50">
         <f t="shared" si="0"/>
-        <v>64.225300000000004</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="3">
+        <v>0.83238145736711278</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51" s="3">
         <v>99</v>
-      </c>
-      <c r="B51" s="3">
-        <v>100</v>
       </c>
       <c r="C51" s="3">
         <v>100</v>
       </c>
-      <c r="E51" s="1"/>
+      <c r="D51" s="3">
+        <v>100</v>
+      </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-      <c r="K51">
+      <c r="H51" s="1"/>
+      <c r="L51">
         <f t="shared" si="0"/>
-        <v>71.025800000000004</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="3">
-        <v>100</v>
+        <v>0.95443588436251059</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1</v>
       </c>
       <c r="B52" s="3">
         <v>100</v>
       </c>
       <c r="C52" s="3">
+        <v>100</v>
+      </c>
+      <c r="D52" s="3">
         <v>94</v>
       </c>
-      <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="K52">
+      <c r="H52" s="1"/>
+      <c r="L52">
         <f t="shared" si="0"/>
-        <v>68.883800000000008</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="3">
+        <v>0.9242399069220143</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53" s="3">
         <v>100</v>
       </c>
-      <c r="B53" s="3">
+      <c r="C53" s="3">
         <v>76</v>
       </c>
-      <c r="C53" s="3">
+      <c r="D53" s="3">
         <v>90</v>
       </c>
-      <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
-      <c r="K53">
+      <c r="H53" s="1"/>
+      <c r="L53">
         <f t="shared" si="0"/>
-        <v>59.091400000000007</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="3">
-        <v>100</v>
+        <v>0.85197802603772754</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1</v>
       </c>
       <c r="B54" s="3">
         <v>100</v>
       </c>
       <c r="C54" s="3">
+        <v>100</v>
+      </c>
+      <c r="D54" s="3">
         <v>92</v>
       </c>
-      <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
-      <c r="K54">
+      <c r="H54" s="1"/>
+      <c r="L54">
         <f t="shared" si="0"/>
-        <v>68.168399999999991</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="3">
+        <v>0.91237621962827264</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55" s="3">
         <v>100</v>
-      </c>
-      <c r="B55" s="3">
-        <v>94</v>
       </c>
       <c r="C55" s="3">
         <v>94</v>
       </c>
-      <c r="E55" s="1"/>
+      <c r="D55" s="3">
+        <v>94</v>
+      </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
-      <c r="K55">
+      <c r="H55" s="1"/>
+      <c r="L55">
         <f t="shared" si="0"/>
-        <v>66.793400000000005</v>
+        <v>0.91627661719602138</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C55">
-    <sortCondition ref="A2:A55"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D55">
+    <sortCondition ref="B2:B55"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>